<commit_message>
scrapping data and writting to excel
</commit_message>
<xml_diff>
--- a/BoProject3/Orders.xlsx
+++ b/BoProject3/Orders.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21320"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0D7EF3A-71C1-4F72-9D2B-B09453A54628}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F9E4E9E-ED0B-4372-AC3C-A7F229E683DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Orders" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>Product</t>
   </si>
@@ -80,13 +80,22 @@
   </si>
   <si>
     <t>Primary Phone</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>Product Does Not Exist</t>
+  </si>
+  <si>
+    <t>Out of Stock</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -398,18 +407,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -423,7 +432,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -432,7 +441,7 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -440,7 +449,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -448,7 +457,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -456,7 +465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -464,7 +473,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -472,7 +481,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -480,12 +489,46 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="1">
         <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3000</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>5000</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -498,21 +541,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1796875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Changed Order Proccess to adapt to Axel's proccess
</commit_message>
<xml_diff>
--- a/BoProject3/Orders.xlsx
+++ b/BoProject3/Orders.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F9E4E9E-ED0B-4372-AC3C-A7F229E683DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{577A453B-3ECD-44F2-82BC-699B42BDCFD8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -413,12 +413,12 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -432,7 +432,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -441,7 +441,7 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -449,7 +449,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -457,7 +457,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -465,7 +465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -473,7 +473,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -481,7 +481,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -489,7 +489,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -503,7 +503,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
@@ -517,7 +517,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -545,17 +545,17 @@
       <selection activeCell="A2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
reading from Google Sheet instead of Excel Sheet
</commit_message>
<xml_diff>
--- a/BoProject3/Orders.xlsx
+++ b/BoProject3/Orders.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C7C842-48FC-4CD5-A362-249DBAB53198}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{365C88DF-280D-4C9A-B142-A54AD6999F42}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -413,12 +413,12 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -432,7 +432,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -441,7 +441,7 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -449,7 +449,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -457,7 +457,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -465,7 +465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -473,7 +473,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -481,7 +481,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -489,7 +489,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -503,7 +503,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
@@ -517,7 +517,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -545,17 +545,17 @@
       <selection activeCell="A2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.08984375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>

</xml_diff>